<commit_message>
Updated Status Summary; Added REFACTOR notes
Marked areas in Square.cs that need Concealed piece clauses added as
well as some major refactoring to condense some hard-coded blocks that
all do similar things.
</commit_message>
<xml_diff>
--- a/dittmar_STATUS_SUMMARY.xlsx
+++ b/dittmar_STATUS_SUMMARY.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G22" sqref="G21:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,16 +639,16 @@
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="21.75" thickTop="1" thickBot="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
       <c r="A9" s="5">
@@ -663,16 +663,16 @@
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>4.2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9"/>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" ht="21.75" thickTop="1" thickBot="1">
       <c r="A11" s="5">
@@ -759,16 +759,16 @@
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="21.75" thickTop="1" thickBot="1">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <v>6</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9"/>
+      <c r="C18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="21.75" thickTop="1" thickBot="1">
       <c r="A19" s="5">

</xml_diff>

<commit_message>
Fixed AI initialization issues.
The AI will now actually play the game using Concealed pieces.  It won't
reveal them, though.
</commit_message>
<xml_diff>
--- a/dittmar_STATUS_SUMMARY.xlsx
+++ b/dittmar_STATUS_SUMMARY.xlsx
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G21:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,16 +831,16 @@
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <v>9.1</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9"/>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
       <c r="A25" s="4">

</xml_diff>